<commit_message>
added Sales Analysis I
</commit_message>
<xml_diff>
--- a/powerBI/sales_analysis/Analytical questions.xlsx
+++ b/powerBI/sales_analysis/Analytical questions.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\mallikarjuna\DSProjects_Temp\powerBI\sales_analysis\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\mallikarjuna\Data_Science\powerBI\sales_analysis\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CCF0B222-2913-491D-80F2-80D1908956F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AB78625-CF61-4EEF-8020-3C058EF19B68}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{B5B9B4C5-ACD1-4D31-92F5-728E4C1256B6}"/>
   </bookViews>
@@ -525,7 +525,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E494583D-81F9-431E-BE24-3CA9C4E631CD}">
-  <dimension ref="A1:I14"/>
+  <dimension ref="A1:I12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -627,11 +627,6 @@
     <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>16</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
-      <c r="H14">
-        <v>1868461</v>
       </c>
     </row>
   </sheetData>

</xml_diff>